<commit_message>
database update Test 1
</commit_message>
<xml_diff>
--- a/daoWeb/src/data/Data.xlsx
+++ b/daoWeb/src/data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\daoAll\daoWeb\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE857EA-5772-4CC6-974A-2D493F022E4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D119C5B-C93E-445A-ACC1-12D3F4FADA5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="580">
   <si>
     <t>Question</t>
   </si>
@@ -1575,15 +1575,239 @@
   <si>
     <t>ID</t>
   </si>
+  <si>
+    <t>Videos</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N8</t>
+  </si>
+  <si>
+    <t>https://youtu.be/8nZDp6OKESs, https://youtu.be/MO-uW1Wm7N8</t>
+  </si>
+  <si>
+    <t>https://youtube.com/shorts/-zeZpYpSIEo</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N9</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N10</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N11</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N12</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N13</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N14</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N15</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N16</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N17</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N18</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N19</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N20</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N21</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N22</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N23</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N24</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N25</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N26</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N27</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N28</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N29</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N30</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N31</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N32</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N33</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N34</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N35</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N36</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N37</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N38</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N39</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N40</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N41</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N42</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N43</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N44</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N45</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N46</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N47</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N48</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N49</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N50</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N51</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N52</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N53</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N54</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N55</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N56</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N57</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N58</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N59</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N60</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N61</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N62</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N63</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N64</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N65</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N66</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N67</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N68</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N69</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N70</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N71</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N72</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N73</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MO-uW1Wm7N74</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1606,13 +1830,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1950,18 +2177,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M71"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>509</v>
       </c>
@@ -2001,8 +2228,11 @@
       <c r="M1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2042,8 +2272,11 @@
       <c r="M2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N2" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2083,8 +2316,11 @@
       <c r="M3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N3" s="1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2124,8 +2360,11 @@
       <c r="M4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N4" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2165,8 +2404,11 @@
       <c r="M5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N5" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2206,8 +2448,11 @@
       <c r="M6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N6" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2247,8 +2492,11 @@
       <c r="M7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N7" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2288,8 +2536,11 @@
       <c r="M8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N8" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2329,8 +2580,11 @@
       <c r="M9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N9" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2370,8 +2624,11 @@
       <c r="M10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N10" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2411,8 +2668,11 @@
       <c r="M11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N11" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2452,8 +2712,11 @@
       <c r="M12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N12" s="1" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2493,8 +2756,11 @@
       <c r="M13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N13" s="1" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2534,8 +2800,11 @@
       <c r="M14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N14" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2575,8 +2844,11 @@
       <c r="M15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N15" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2616,8 +2888,11 @@
       <c r="M16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N16" s="1" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2657,8 +2932,11 @@
       <c r="M17" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N17" s="1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2698,8 +2976,11 @@
       <c r="M18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N18" s="1" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2739,8 +3020,11 @@
       <c r="M19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N19" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2780,8 +3064,11 @@
       <c r="M20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N20" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2821,8 +3108,11 @@
       <c r="M21" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N21" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2862,8 +3152,11 @@
       <c r="M22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N22" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2903,8 +3196,11 @@
       <c r="M23" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N23" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2944,8 +3240,11 @@
       <c r="M24" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N24" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2985,8 +3284,11 @@
       <c r="M25" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N25" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3026,8 +3328,11 @@
       <c r="M26" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N26" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3067,8 +3372,11 @@
       <c r="M27" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N27" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3108,8 +3416,11 @@
       <c r="M28" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N28" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3149,8 +3460,11 @@
       <c r="M29" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N29" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3190,8 +3504,11 @@
       <c r="M30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N30" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3231,8 +3548,11 @@
       <c r="M31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N31" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3272,8 +3592,11 @@
       <c r="M32" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N32" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3313,8 +3636,11 @@
       <c r="M33" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N33" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3354,8 +3680,11 @@
       <c r="M34" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N34" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3395,8 +3724,11 @@
       <c r="M35" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N35" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3436,8 +3768,11 @@
       <c r="M36" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N36" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3477,8 +3812,11 @@
       <c r="M37" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N37" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3518,8 +3856,11 @@
       <c r="M38" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N38" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3559,8 +3900,11 @@
       <c r="M39" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N39" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3600,8 +3944,11 @@
       <c r="M40" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N40" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3641,8 +3988,11 @@
       <c r="M41" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N41" s="1" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3682,8 +4032,11 @@
       <c r="M42" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N42" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3723,8 +4076,11 @@
       <c r="M43" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N43" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3764,8 +4120,11 @@
       <c r="M44" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N44" s="1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3805,8 +4164,11 @@
       <c r="M45" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N45" s="1" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3846,8 +4208,11 @@
       <c r="M46" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N46" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3887,8 +4252,11 @@
       <c r="M47" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N47" s="1" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3928,8 +4296,11 @@
       <c r="M48" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N48" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3969,8 +4340,11 @@
       <c r="M49" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N49" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4010,8 +4384,11 @@
       <c r="M50" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N50" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4051,8 +4428,11 @@
       <c r="M51" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N51" s="1" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4092,8 +4472,11 @@
       <c r="M52" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N52" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4133,8 +4516,11 @@
       <c r="M53" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N53" s="1" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4174,8 +4560,11 @@
       <c r="M54" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N54" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4215,8 +4604,11 @@
       <c r="M55" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N55" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4256,8 +4648,11 @@
       <c r="M56" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N56" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4297,8 +4692,11 @@
       <c r="M57" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N57" s="1" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4338,8 +4736,11 @@
       <c r="M58" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N58" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4379,8 +4780,11 @@
       <c r="M59" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N59" s="1" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4420,8 +4824,11 @@
       <c r="M60" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N60" s="1" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4461,8 +4868,11 @@
       <c r="M61" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N61" s="1" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4502,8 +4912,11 @@
       <c r="M62" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N62" s="1" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4543,8 +4956,11 @@
       <c r="M63" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N63" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4584,8 +5000,11 @@
       <c r="M64" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N64" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4625,8 +5044,11 @@
       <c r="M65" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N65" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4666,8 +5088,11 @@
       <c r="M66" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N66" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4707,8 +5132,11 @@
       <c r="M67" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N67" s="1" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4748,8 +5176,11 @@
       <c r="M68" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N68" s="1" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4789,8 +5220,11 @@
       <c r="M69" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N69" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4830,8 +5264,11 @@
       <c r="M70" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N70" s="1" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4871,8 +5308,19 @@
       <c r="M71" t="s">
         <v>29</v>
       </c>
+      <c r="N71" s="1" t="s">
+        <v>579</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="N3" r:id="rId1" display="https://youtu.be/8nZDp6OKESs, " xr:uid="{64CE10BB-9A43-410F-B494-C2312B753965}"/>
+    <hyperlink ref="N2" r:id="rId2" xr:uid="{3C554EC2-C25A-40ED-A8E5-E0279635D318}"/>
+    <hyperlink ref="N4" r:id="rId3" xr:uid="{43EEAE05-F88C-41A9-96FB-94A7EAAF279A}"/>
+    <hyperlink ref="N5" r:id="rId4" xr:uid="{D8C03376-B314-4BDE-8A5D-442E6B4417FE}"/>
+    <hyperlink ref="N6:N71" r:id="rId5" display="https://youtu.be/MO-uW1Wm7N8" xr:uid="{C3B6B8D1-8D5A-477D-967C-584099B033B9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A2:M6 A8:M71 A7:L7 B1:M1" numberStoredAsText="1"/>

</xml_diff>